<commit_message>
Character Data in json format
</commit_message>
<xml_diff>
--- a/data/Genshin Impact Data.xlsx
+++ b/data/Genshin Impact Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HomeFiles\Github\cool-apps\genshin-crafting-table\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5536D663-2C11-4A42-93B4-E790DEF8A518}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81625BF-AC1B-4009-ABAF-9F37A8F4DD1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{786E68F0-8863-4571-A8DF-93FEE407AF97}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{786E68F0-8863-4571-A8DF-93FEE407AF97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="69">
   <si>
     <t>GENSHIN DATA</t>
   </si>
@@ -232,13 +232,22 @@
   </si>
   <si>
     <t>Energy Recharge: 100%</t>
+  </si>
+  <si>
+    <t>Max Stamina: 240</t>
+  </si>
+  <si>
+    <t>Max HP</t>
+  </si>
+  <si>
+    <t>(Base HP * HP% (Weapon, Artifact, Ascension)) + Flat MAX HP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,6 +280,14 @@
     <font>
       <b/>
       <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -325,7 +342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -360,6 +377,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -676,20 +701,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E30B7E8B-3911-4AD7-A866-39BF1884B242}">
-  <dimension ref="A1:Y377"/>
+  <dimension ref="A1:AB377"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A341" workbookViewId="0">
-      <selection activeCell="O357" sqref="O357"/>
+    <sheetView tabSelected="1" topLeftCell="A348" workbookViewId="0">
+      <selection activeCell="E366" sqref="E366:H377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:28" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
@@ -705,19 +730,22 @@
       <c r="H3" t="s">
         <v>65</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" t="s">
+        <v>66</v>
+      </c>
+      <c r="N3" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="L4" t="s">
+      <c r="O4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>3</v>
       </c>
@@ -733,12 +761,9 @@
       <c r="H5" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="P5" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
@@ -748,8 +773,11 @@
       <c r="W5" s="12"/>
       <c r="X5" s="12"/>
       <c r="Y5" s="12"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="12"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>1</v>
       </c>
@@ -765,12 +793,9 @@
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="P6" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
       <c r="Q6" s="12"/>
       <c r="R6" s="12"/>
       <c r="S6" s="12"/>
@@ -780,8 +805,11 @@
       <c r="W6" s="12"/>
       <c r="X6" s="12"/>
       <c r="Y6" s="12"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>20</v>
       </c>
@@ -797,9 +825,6 @@
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
       <c r="P7" s="12"/>
       <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
@@ -810,8 +835,11 @@
       <c r="W7" s="12"/>
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
-    </row>
-    <row r="8" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="12"/>
+    </row>
+    <row r="8" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>8</v>
       </c>
@@ -827,11 +855,11 @@
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="L8" t="s">
+      <c r="O8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>40</v>
       </c>
@@ -847,16 +875,16 @@
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="M9" s="11" t="s">
+      <c r="P9" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
       <c r="Q9" s="11"/>
       <c r="R9" s="11"/>
-    </row>
-    <row r="10" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+    </row>
+    <row r="10" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>9</v>
       </c>
@@ -873,7 +901,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>50</v>
       </c>
@@ -889,11 +917,11 @@
       <c r="H11" s="4">
         <v>0.06</v>
       </c>
-      <c r="L11" t="s">
+      <c r="O11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>10</v>
       </c>
@@ -909,11 +937,11 @@
       <c r="H12" s="6">
         <v>0.12</v>
       </c>
-      <c r="M12" s="13" t="s">
+      <c r="P12" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>60</v>
       </c>
@@ -930,7 +958,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>11</v>
       </c>
@@ -946,8 +974,11 @@
       <c r="H14" s="4">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>70</v>
       </c>
@@ -963,8 +994,23 @@
       <c r="H15" s="4">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P15" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="18"/>
+      <c r="Z15" s="18"/>
+      <c r="AA15" s="18"/>
+      <c r="AB15" s="18"/>
+    </row>
+    <row r="16" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>12</v>
       </c>
@@ -981,7 +1027,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>80</v>
       </c>
@@ -997,13 +1043,37 @@
       <c r="H17" s="6">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N17" s="16"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="O18" s="12"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+      <c r="Y19" s="17"/>
+      <c r="Z19" s="17"/>
+      <c r="AA19" s="17"/>
+      <c r="AB19" s="17"/>
+    </row>
+    <row r="20" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>3</v>
       </c>
@@ -1020,7 +1090,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>1</v>
       </c>
@@ -1037,7 +1107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="C22">
         <v>20</v>
@@ -1055,7 +1125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>8</v>
       </c>
@@ -1072,7 +1142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>40</v>
       </c>
@@ -1089,7 +1159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>9</v>
       </c>
@@ -1106,7 +1176,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26">
         <v>50</v>
       </c>
@@ -1123,7 +1193,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>10</v>
       </c>
@@ -1140,7 +1210,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>60</v>
       </c>
@@ -1157,7 +1227,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
         <v>11</v>
       </c>
@@ -1174,7 +1244,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30">
         <v>70</v>
       </c>
@@ -1191,7 +1261,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
         <v>12</v>
       </c>
@@ -1208,7 +1278,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32">
         <v>80</v>
       </c>
@@ -2173,13 +2243,13 @@
         <v>20</v>
       </c>
       <c r="E97" s="2">
-        <v>2237</v>
+        <v>2621</v>
       </c>
       <c r="F97" s="3">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="G97" s="3">
-        <v>113</v>
+        <v>158</v>
       </c>
       <c r="H97" s="4">
         <v>0.05</v>
@@ -2189,14 +2259,14 @@
       <c r="C98" t="s">
         <v>8</v>
       </c>
-      <c r="E98" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>23</v>
+      <c r="E98" s="5">
+        <v>3488</v>
+      </c>
+      <c r="F98" s="1">
+        <v>90</v>
+      </c>
+      <c r="G98" s="1">
+        <v>211</v>
       </c>
       <c r="H98" s="6">
         <v>0.05</v>
@@ -2568,17 +2638,17 @@
       <c r="C122">
         <v>80</v>
       </c>
-      <c r="E122" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F122" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G122" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H122" s="1" t="s">
-        <v>23</v>
+      <c r="E122" s="5">
+        <v>8481</v>
+      </c>
+      <c r="F122" s="1">
+        <v>188</v>
+      </c>
+      <c r="G122" s="1">
+        <v>532</v>
+      </c>
+      <c r="H122" s="8">
+        <v>0.18</v>
       </c>
     </row>
     <row r="124" spans="2:8" x14ac:dyDescent="0.25">
@@ -6280,10 +6350,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="M5:Y5"/>
-    <mergeCell ref="M6:Y6"/>
-    <mergeCell ref="M7:Y7"/>
+  <mergeCells count="2">
+    <mergeCell ref="O19:AB19"/>
+    <mergeCell ref="P15:AB15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>